<commit_message>
add method for comm
</commit_message>
<xml_diff>
--- a/src/test/resources/commeq.xlsx
+++ b/src/test/resources/commeq.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyData\pliki do testow\practice\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F6A022-FFE2-47FE-B594-FA41F96EB24A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="185"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="34">
   <si>
     <t>NET_STATION_ID</t>
   </si>
@@ -78,58 +72,62 @@
     <t>PLC</t>
   </si>
   <si>
-    <t>rom1</t>
-  </si>
-  <si>
-    <t>rom2</t>
-  </si>
-  <si>
-    <t>rom3</t>
-  </si>
-  <si>
-    <t>rom4</t>
-  </si>
-  <si>
-    <t>rom5</t>
-  </si>
-  <si>
-    <t>rom6</t>
-  </si>
-  <si>
-    <t>rom7</t>
-  </si>
-  <si>
-    <t>rom8</t>
-  </si>
-  <si>
-    <t>rom9</t>
-  </si>
-  <si>
-    <t>rom10</t>
-  </si>
-  <si>
-    <t>rom11</t>
-  </si>
-  <si>
-    <t>rom12</t>
-  </si>
-  <si>
-    <t>rom13</t>
-  </si>
-  <si>
-    <t>rom14</t>
-  </si>
-  <si>
     <t>Stage_2_WN</t>
   </si>
   <si>
     <t>2019-12-06</t>
+  </si>
+  <si>
+    <t>gga</t>
+  </si>
+  <si>
+    <t>Auto2020-02-06-6978</t>
+  </si>
+  <si>
+    <t>Auto2020-02-06-6709</t>
+  </si>
+  <si>
+    <t>Auto2020-02-06-8166</t>
+  </si>
+  <si>
+    <t>Auto2020-02-06-6877</t>
+  </si>
+  <si>
+    <t>Auto2020-02-06-4736</t>
+  </si>
+  <si>
+    <t>Auto2020-02-06-5273</t>
+  </si>
+  <si>
+    <t>Auto2020-02-06-3194</t>
+  </si>
+  <si>
+    <t>Auto2020-02-06-6478</t>
+  </si>
+  <si>
+    <t>Auto2020-02-06-5578</t>
+  </si>
+  <si>
+    <t>Auto2020-02-06-5701</t>
+  </si>
+  <si>
+    <t>Auto2020-02-06-1499</t>
+  </si>
+  <si>
+    <t>Auto2020-02-06-8967</t>
+  </si>
+  <si>
+    <t>Auto2020-02-06-513</t>
+  </si>
+  <si>
+    <t>Auto2020-02-06-796</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -183,7 +181,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -460,26 +458,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3:K15"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="32.33203125" customWidth="1"/>
-    <col min="4" max="4" width="28.6640625" customWidth="1"/>
-    <col min="5" max="5" width="27.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.44140625" customWidth="1"/>
-    <col min="11" max="11" width="25.6640625" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.6640625" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="25.0" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="32.33203125" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="28.6640625" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="27.5546875" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="32.0" collapsed="false"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="24.5546875" collapsed="false"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="30.5546875" collapsed="false"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="15.6640625" collapsed="false"/>
+    <col min="10" max="10" customWidth="true" width="17.44140625" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" width="25.6640625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -519,7 +517,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="3" t="s">
@@ -544,7 +542,7 @@
         <v>15</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>16</v>
@@ -552,7 +550,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="3" t="s">
@@ -577,7 +575,7 @@
         <v>15</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>16</v>
@@ -585,7 +583,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>11</v>
@@ -609,7 +607,7 @@
         <v>15</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>16</v>
@@ -617,7 +615,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>11</v>
@@ -641,7 +639,7 @@
         <v>15</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>16</v>
@@ -649,7 +647,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>11</v>
@@ -673,7 +671,7 @@
         <v>15</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>16</v>
@@ -681,7 +679,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>11</v>
@@ -705,7 +703,7 @@
         <v>15</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>16</v>
@@ -713,7 +711,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>11</v>
@@ -737,7 +735,7 @@
         <v>15</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>16</v>
@@ -745,7 +743,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>11</v>
@@ -769,7 +767,7 @@
         <v>15</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>16</v>
@@ -777,7 +775,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>11</v>
@@ -801,7 +799,7 @@
         <v>15</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>16</v>
@@ -809,7 +807,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>11</v>
@@ -833,7 +831,7 @@
         <v>15</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>16</v>
@@ -841,7 +839,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>11</v>
@@ -862,10 +860,10 @@
         <v>3163</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>16</v>
@@ -873,7 +871,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>11</v>
@@ -894,10 +892,10 @@
         <v>3164</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>16</v>
@@ -905,7 +903,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>11</v>
@@ -926,10 +924,10 @@
         <v>3165</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>16</v>
@@ -937,7 +935,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>11</v>
@@ -958,10 +956,10 @@
         <v>3166</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>16</v>

</xml_diff>